<commit_message>
update Readme xlsx for introducing pip packages
Signed-off-by: Sprindy Liu <sprindy.liu@gmail.com>
</commit_message>
<xml_diff>
--- a/Documents/Readme.xlsx
+++ b/Documents/Readme.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\3_code\python\python_study\python_from_0_to_0.1\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8EC6F59-059E-47FD-9F98-F8330BF51770}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B12CE7DE-C073-47FD-9F69-C1AC52C41C3D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2925" yWindow="2475" windowWidth="24210" windowHeight="11670" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2925" yWindow="2475" windowWidth="24210" windowHeight="11670" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Resources" sheetId="3" r:id="rId1"/>
     <sheet name="Schedule" sheetId="2" r:id="rId2"/>
     <sheet name="Attendees" sheetId="1" r:id="rId3"/>
     <sheet name="Tools" sheetId="4" r:id="rId4"/>
+    <sheet name="pip" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,23 +29,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="145">
   <si>
     <t xml:space="preserve">想高效分析客户数据, 提高查询调取数据效率，减少重复操作，提高数据的整洁和目标导向性. </t>
   </si>
   <si>
-    <t>行业</t>
-  </si>
-  <si>
-    <t>职业</t>
-  </si>
-  <si>
-    <t>电脑系统</t>
-  </si>
-  <si>
-    <t>（任何编程语言）编程基础</t>
-  </si>
-  <si>
     <t>为啥想学Python？</t>
   </si>
   <si>
@@ -387,9 +376,6 @@
     <t>Download Address</t>
   </si>
   <si>
-    <t>brew install python3</t>
-  </si>
-  <si>
     <t>https://code.visualstudio.com/Download</t>
   </si>
   <si>
@@ -400,6 +386,84 @@
   </si>
   <si>
     <t>PPT for every lesson will be included</t>
+  </si>
+  <si>
+    <t>python3 -m pip install openpyxl</t>
+  </si>
+  <si>
+    <t>python3 -m pip install -U pylint --user</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>install command</t>
+  </si>
+  <si>
+    <t>ModuleNotFoundError: No module named 'openpyxl'</t>
+  </si>
+  <si>
+    <t>Error Message</t>
+  </si>
+  <si>
+    <t>python3 -m pip install --upgrade pip</t>
+  </si>
+  <si>
+    <t>install pylint</t>
+  </si>
+  <si>
+    <t>for read and write xlsx file</t>
+  </si>
+  <si>
+    <t>python3 -m pip install pandas</t>
+  </si>
+  <si>
+    <t>python3 -m pip install matplotlib</t>
+  </si>
+  <si>
+    <t>pandas</t>
+  </si>
+  <si>
+    <t>matplotlib</t>
+  </si>
+  <si>
+    <t>ImportError: Missing optional dependency 'xlrd'. Install xlrd &gt;= 1.0.0 for Excel support Use pip or conda to install xlrd.</t>
+  </si>
+  <si>
+    <t>python3 -m pip install xlrd</t>
+  </si>
+  <si>
+    <t>for read xlsx file</t>
+  </si>
+  <si>
+    <t>xlsx</t>
+  </si>
+  <si>
+    <t>plot</t>
+  </si>
+  <si>
+    <t>pip</t>
+  </si>
+  <si>
+    <t>visual studio code</t>
+  </si>
+  <si>
+    <t>Pylint is a Python static code analysis tool which looks for programming errors,helps enforcing a coding standard, sniffs for code smells and offers simple refactoringsuggestions.</t>
+  </si>
+  <si>
+    <t>update pip itself, pip is the package installer for Python. You can use pip to install packages from the Python Package Index and other indexes.</t>
+  </si>
+  <si>
+    <t>Industry</t>
+  </si>
+  <si>
+    <t>Occupation</t>
+  </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>Programing Experience</t>
   </si>
 </sst>
 </file>
@@ -465,7 +529,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -479,6 +543,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -764,8 +831,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B267E06-A0EE-4A60-A105-2224F1953C65}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -777,40 +844,40 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" s="1" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -820,17 +887,17 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
       <c r="B7" s="3" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C7" s="1"/>
     </row>
@@ -841,19 +908,19 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C9" s="1"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B11" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -889,52 +956,52 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>82</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -942,11 +1009,11 @@
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
       <c r="B4" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -954,11 +1021,11 @@
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
       <c r="B5" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -966,11 +1033,11 @@
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
       <c r="B6" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -978,25 +1045,25 @@
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -1004,11 +1071,11 @@
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
@@ -1016,11 +1083,11 @@
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
       <c r="B10" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
@@ -1028,25 +1095,25 @@
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
@@ -1054,11 +1121,11 @@
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
@@ -1078,8 +1145,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1095,28 +1162,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D1" t="s">
+        <v>142</v>
+      </c>
+      <c r="E1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F1" t="s">
+        <v>144</v>
+      </c>
+      <c r="G1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
       <c r="H1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1124,22 +1191,22 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="G2" t="s">
         <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1147,19 +1214,19 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" t="s">
         <v>13</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1167,22 +1234,22 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" t="s">
         <v>18</v>
       </c>
-      <c r="C4" t="s">
+      <c r="G4" t="s">
         <v>19</v>
-      </c>
-      <c r="D4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1190,10 +1257,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="G5" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1201,19 +1268,19 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" t="s">
         <v>26</v>
       </c>
-      <c r="C6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" t="s">
-        <v>30</v>
-      </c>
       <c r="F6" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="G6" t="s">
         <v>0</v>
@@ -1224,19 +1291,19 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D7" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F7" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="G7" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1244,13 +1311,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="F8" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="G8" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1258,22 +1325,22 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" t="s">
         <v>38</v>
       </c>
-      <c r="C9" t="s">
+      <c r="G9" t="s">
         <v>39</v>
-      </c>
-      <c r="D9" t="s">
-        <v>40</v>
-      </c>
-      <c r="E9" t="s">
-        <v>41</v>
-      </c>
-      <c r="F9" t="s">
-        <v>42</v>
-      </c>
-      <c r="G9" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1281,22 +1348,22 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" t="s">
+        <v>43</v>
+      </c>
+      <c r="G10" t="s">
         <v>44</v>
-      </c>
-      <c r="C10" t="s">
-        <v>58</v>
-      </c>
-      <c r="D10" t="s">
-        <v>45</v>
-      </c>
-      <c r="E10" t="s">
-        <v>46</v>
-      </c>
-      <c r="F10" t="s">
-        <v>47</v>
-      </c>
-      <c r="G10" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -1304,16 +1371,16 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D11" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F11" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="G11" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1321,10 +1388,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="G12" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1332,16 +1399,16 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D13" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="F13" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="G13" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1349,19 +1416,19 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C14" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D14" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E14" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="G14" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1369,19 +1436,19 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C15" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D15" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E15" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="G15" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -1393,8 +1460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAD68CDF-6082-404F-9587-CC31EF4E1743}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1410,26 +1477,26 @@
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="6" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C1" s="6"/>
       <c r="D1" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -1437,68 +1504,68 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>116</v>
+        <v>108</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>109</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="3" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="3" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -1510,9 +1577,139 @@
   <hyperlinks>
     <hyperlink ref="F3" r:id="rId1" xr:uid="{E45FF947-6BE2-461F-A3E2-E18536134EE9}"/>
     <hyperlink ref="F4" r:id="rId2" xr:uid="{54CEF991-5998-4C51-A660-039789751FE8}"/>
-    <hyperlink ref="B3" r:id="rId3" xr:uid="{323AEF15-BB18-4478-AE19-56719F68495B}"/>
-    <hyperlink ref="C3" r:id="rId4" xr:uid="{C529D924-59FB-43A3-8F66-DD90C277593B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5DE38A3-6ACA-4B04-886E-9C5C02EA135E}">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="52.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="C4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D4" t="s">
+        <v>127</v>
+      </c>
+      <c r="E4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" t="s">
+        <v>133</v>
+      </c>
+      <c r="D5" t="s">
+        <v>134</v>
+      </c>
+      <c r="E5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="C6" t="s">
+        <v>128</v>
+      </c>
+      <c r="D6" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="7"/>
+      <c r="C7" t="s">
+        <v>129</v>
+      </c>
+      <c r="D7" t="s">
+        <v>131</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B6:B7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update guideline website for the plots
pandas/matplotlib/beaborn

Signed-off-by: Sprindy Liu <sprindy_liu@icloud.com>
</commit_message>
<xml_diff>
--- a/Documents/Readme.xlsx
+++ b/Documents/Readme.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11208"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\3_code\python\python_study\python_from_0_to_0.1\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Sprindy/program/python/python_from_0_to_0.1/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B12CE7DE-C073-47FD-9F69-C1AC52C41C3D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A17B1F3C-E57F-B441-8EDC-CA367DDA0C3C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2925" yWindow="2475" windowWidth="24210" windowHeight="11670" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1380" yWindow="2480" windowWidth="24220" windowHeight="11680" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Resources" sheetId="3" r:id="rId1"/>
     <sheet name="Schedule" sheetId="2" r:id="rId2"/>
     <sheet name="Attendees" sheetId="1" r:id="rId3"/>
     <sheet name="Tools" sheetId="4" r:id="rId4"/>
-    <sheet name="pip" sheetId="5" r:id="rId5"/>
+    <sheet name="Pip" sheetId="5" r:id="rId5"/>
+    <sheet name="Plot" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="154">
   <si>
     <t xml:space="preserve">想高效分析客户数据, 提高查询调取数据效率，减少重复操作，提高数据的整洁和目标导向性. </t>
   </si>
@@ -464,6 +465,33 @@
   </si>
   <si>
     <t>Programing Experience</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>https://pandas.pydata.org/docs/reference/frame.html</t>
+  </si>
+  <si>
+    <t>https://matplotlib.org</t>
+  </si>
+  <si>
+    <t>reference tutorials</t>
+  </si>
+  <si>
+    <t>seaborn</t>
+  </si>
+  <si>
+    <t>python3 -m pip install seaborn</t>
+  </si>
+  <si>
+    <t>https://seaborn.pydata.org</t>
+  </si>
+  <si>
+    <t>Categrory</t>
+  </si>
+  <si>
+    <t>name</t>
   </si>
 </sst>
 </file>
@@ -529,7 +557,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -546,8 +574,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -835,14 +867,14 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14" style="2" customWidth="1"/>
-    <col min="2" max="2" width="53.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="47.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>91</v>
       </c>
@@ -853,7 +885,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>88</v>
       </c>
@@ -862,14 +894,14 @@
       </c>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="5"/>
       <c r="B3" s="1" t="s">
         <v>118</v>
       </c>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>87</v>
       </c>
@@ -880,12 +912,12 @@
         <v>117</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="5"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>89</v>
       </c>
@@ -894,19 +926,19 @@
       </c>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="5"/>
       <c r="B7" s="3" t="s">
         <v>84</v>
       </c>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="4"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>90</v>
       </c>
@@ -915,7 +947,7 @@
       </c>
       <c r="C9" s="1"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>116</v>
       </c>
@@ -946,15 +978,15 @@
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="13.28515625" customWidth="1"/>
-    <col min="5" max="5" width="29.140625" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.33203125" customWidth="1"/>
+    <col min="5" max="5" width="29.1640625" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>82</v>
       </c>
@@ -974,7 +1006,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>73</v>
       </c>
@@ -992,7 +1024,7 @@
       </c>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="6"/>
       <c r="B3" s="1" t="s">
         <v>62</v>
@@ -1006,7 +1038,7 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="6"/>
       <c r="B4" s="1" t="s">
         <v>63</v>
@@ -1018,7 +1050,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="6"/>
       <c r="B5" s="1" t="s">
         <v>64</v>
@@ -1030,7 +1062,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="6"/>
       <c r="B6" s="1" t="s">
         <v>65</v>
@@ -1042,7 +1074,7 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="6"/>
       <c r="B7" s="1" t="s">
         <v>66</v>
@@ -1054,7 +1086,7 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>77</v>
       </c>
@@ -1068,7 +1100,7 @@
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="6"/>
       <c r="B9" s="1" t="s">
         <v>68</v>
@@ -1080,7 +1112,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="6"/>
       <c r="B10" s="1" t="s">
         <v>69</v>
@@ -1092,7 +1124,7 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="6"/>
       <c r="B11" s="1" t="s">
         <v>70</v>
@@ -1104,7 +1136,7 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>81</v>
       </c>
@@ -1118,7 +1150,7 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="6"/>
       <c r="B13" s="1" t="s">
         <v>72</v>
@@ -1149,18 +1181,18 @@
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" customWidth="1"/>
-    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.33203125" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.85546875" customWidth="1"/>
+    <col min="5" max="5" width="28.83203125" customWidth="1"/>
     <col min="6" max="6" width="39" customWidth="1"/>
-    <col min="7" max="7" width="114.42578125" customWidth="1"/>
-    <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="114.5" customWidth="1"/>
+    <col min="8" max="8" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1186,7 +1218,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1209,7 +1241,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1229,7 +1261,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1252,7 +1284,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1263,7 +1295,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1286,7 +1318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1306,7 +1338,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1320,7 +1352,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1343,7 +1375,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1366,7 +1398,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1383,7 +1415,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1394,7 +1426,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1411,7 +1443,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1431,7 +1463,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1460,21 +1492,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAD68CDF-6082-404F-9587-CC31EF4E1743}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" customWidth="1"/>
-    <col min="4" max="4" width="20.140625" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="44.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" customWidth="1"/>
+    <col min="4" max="4" width="20.1640625" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="44.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="6" t="s">
         <v>101</v>
@@ -1490,7 +1522,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>104</v>
@@ -1502,7 +1534,7 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>108</v>
       </c>
@@ -1520,7 +1552,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>103</v>
       </c>
@@ -1538,7 +1570,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>106</v>
       </c>
@@ -1554,7 +1586,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>107</v>
       </c>
@@ -1565,7 +1597,7 @@
         <v>110</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>110</v>
+        <v>145</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -1584,26 +1616,26 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5DE38A3-6ACA-4B04-886E-9C5C02EA135E}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="52.28515625" customWidth="1"/>
+    <col min="2" max="2" width="17" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="52.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>91</v>
       </c>
       <c r="C1" t="s">
@@ -1616,11 +1648,11 @@
         <v>124</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>137</v>
       </c>
       <c r="C2" t="s">
@@ -1630,11 +1662,11 @@
         <v>140</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>138</v>
       </c>
       <c r="C3" t="s">
@@ -1647,11 +1679,11 @@
         <v>139</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="8" t="s">
         <v>135</v>
       </c>
       <c r="C4" t="s">
@@ -1664,11 +1696,11 @@
         <v>123</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="7"/>
+      <c r="B5" s="8"/>
       <c r="C5" t="s">
         <v>133</v>
       </c>
@@ -1679,11 +1711,11 @@
         <v>132</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="8" t="s">
         <v>136</v>
       </c>
       <c r="C6" t="s">
@@ -1693,23 +1725,96 @@
         <v>130</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" s="7"/>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B7" s="8"/>
       <c r="C7" t="s">
         <v>129</v>
       </c>
       <c r="D7" t="s">
         <v>131</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" s="8"/>
+      <c r="C8" t="s">
+        <v>150</v>
+      </c>
+      <c r="D8" t="s">
+        <v>149</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B6:B8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D94782C-BCB3-5144-841C-41597F5E6A34}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="43" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="B2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="7"/>
+      <c r="B3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="7"/>
+      <c r="B4" t="s">
+        <v>149</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>151</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:A4"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C4" r:id="rId1" xr:uid="{7E2BFCC3-BE60-514D-AF5E-FEB64486F0CC}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add python xlsx rw module tutorial.
Signed-off-by: Sprindy Liu <sprindy_liu@icloud.com>
</commit_message>
<xml_diff>
--- a/Documents/Readme.xlsx
+++ b/Documents/Readme.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Sprindy/program/python/python_from_0_to_0.1/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A17B1F3C-E57F-B441-8EDC-CA367DDA0C3C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5F0D9EE-2A00-D341-AD01-360815C6D074}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1380" yWindow="2480" windowWidth="24220" windowHeight="11680" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="156">
   <si>
     <t xml:space="preserve">想高效分析客户数据, 提高查询调取数据效率，减少重复操作，提高数据的整洁和目标导向性. </t>
   </si>
@@ -492,6 +492,12 @@
   </si>
   <si>
     <t>name</t>
+  </si>
+  <si>
+    <t>https://openpyxl.readthedocs.io/en/default/</t>
+  </si>
+  <si>
+    <t>openpyxl</t>
   </si>
 </sst>
 </file>
@@ -567,6 +573,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -574,12 +581,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -886,7 +892,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="6" t="s">
         <v>88</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -895,14 +901,14 @@
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="5"/>
+      <c r="A3" s="6"/>
       <c r="B3" s="1" t="s">
         <v>118</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="6" t="s">
         <v>87</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -913,12 +919,12 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="5"/>
+      <c r="A5" s="6"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="6" t="s">
         <v>89</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -927,7 +933,7 @@
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="5"/>
+      <c r="A7" s="6"/>
       <c r="B7" s="3" t="s">
         <v>84</v>
       </c>
@@ -1007,7 +1013,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="7" t="s">
         <v>73</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1025,7 +1031,7 @@
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="6"/>
+      <c r="A3" s="7"/>
       <c r="B3" s="1" t="s">
         <v>62</v>
       </c>
@@ -1039,7 +1045,7 @@
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="6"/>
+      <c r="A4" s="7"/>
       <c r="B4" s="1" t="s">
         <v>63</v>
       </c>
@@ -1051,7 +1057,7 @@
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="6"/>
+      <c r="A5" s="7"/>
       <c r="B5" s="1" t="s">
         <v>64</v>
       </c>
@@ -1063,7 +1069,7 @@
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="6"/>
+      <c r="A6" s="7"/>
       <c r="B6" s="1" t="s">
         <v>65</v>
       </c>
@@ -1075,7 +1081,7 @@
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="6"/>
+      <c r="A7" s="7"/>
       <c r="B7" s="1" t="s">
         <v>66</v>
       </c>
@@ -1087,7 +1093,7 @@
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="7" t="s">
         <v>77</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -1101,7 +1107,7 @@
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="6"/>
+      <c r="A9" s="7"/>
       <c r="B9" s="1" t="s">
         <v>68</v>
       </c>
@@ -1113,7 +1119,7 @@
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="6"/>
+      <c r="A10" s="7"/>
       <c r="B10" s="1" t="s">
         <v>69</v>
       </c>
@@ -1125,7 +1131,7 @@
       <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="6"/>
+      <c r="A11" s="7"/>
       <c r="B11" s="1" t="s">
         <v>70</v>
       </c>
@@ -1137,7 +1143,7 @@
       <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="7" t="s">
         <v>81</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1151,7 +1157,7 @@
       <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="6"/>
+      <c r="A13" s="7"/>
       <c r="B13" s="1" t="s">
         <v>72</v>
       </c>
@@ -1508,10 +1514,10 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="C1" s="6"/>
+      <c r="C1" s="7"/>
       <c r="D1" s="1" t="s">
         <v>102</v>
       </c>
@@ -1757,10 +1763,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D94782C-BCB3-5144-841C-41597F5E6A34}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1780,7 +1786,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="9" t="s">
         <v>136</v>
       </c>
       <c r="B2" t="s">
@@ -1791,7 +1797,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="7"/>
+      <c r="A3" s="9"/>
       <c r="B3" t="s">
         <v>131</v>
       </c>
@@ -1800,12 +1806,23 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="7"/>
+      <c r="A4" s="9"/>
       <c r="B4" t="s">
         <v>149</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="5" t="s">
         <v>151</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>135</v>
+      </c>
+      <c r="B5" t="s">
+        <v>155</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -1814,6 +1831,7 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C4" r:id="rId1" xr:uid="{7E2BFCC3-BE60-514D-AF5E-FEB64486F0CC}"/>
+    <hyperlink ref="C5" r:id="rId2" xr:uid="{ED80F6DB-712C-E843-AAE7-CC267FC0FD64}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add more for Readme.xlsx
use -i to set server adderss to speed up download

Signed-off-by: Sprindy Liu <sprindy_liu@icloud.com>
</commit_message>
<xml_diff>
--- a/Documents/Readme.xlsx
+++ b/Documents/Readme.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Sprindy/program/python/python_from_0_to_0.1/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5F0D9EE-2A00-D341-AD01-360815C6D074}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C67A7BEB-3B50-834F-9955-EF434D946EB1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1380" yWindow="2480" windowWidth="24220" windowHeight="11680" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1740" windowWidth="24220" windowHeight="11680" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Resources" sheetId="3" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="164">
   <si>
     <t xml:space="preserve">想高效分析客户数据, 提高查询调取数据效率，减少重复操作，提高数据的整洁和目标导向性. </t>
   </si>
@@ -498,6 +498,30 @@
   </si>
   <si>
     <t>openpyxl</t>
+  </si>
+  <si>
+    <t>python3 -m pip install BeautifulSoup4</t>
+  </si>
+  <si>
+    <t>python3 -m pip install Scrapy</t>
+  </si>
+  <si>
+    <t>python3 -m pip install -i https://pypi.tuna.tsinghua.edu.cn/simple fake_useragent</t>
+  </si>
+  <si>
+    <t>http://www.sqliteexpert.com/download.html</t>
+  </si>
+  <si>
+    <t>https://sqlitebrowser.org/blog/version-3-11-2-released/</t>
+  </si>
+  <si>
+    <t>sqlite</t>
+  </si>
+  <si>
+    <t>指定国内的服务器，速度更快</t>
+  </si>
+  <si>
+    <t>爬虫</t>
   </si>
 </sst>
 </file>
@@ -535,7 +559,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -558,12 +582,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -581,10 +616,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1496,10 +1532,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAD68CDF-6082-404F-9587-CC31EF4E1743}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1608,6 +1644,23 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="D7" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F8" s="5"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:C1"/>
@@ -1615,6 +1668,8 @@
   <hyperlinks>
     <hyperlink ref="F3" r:id="rId1" xr:uid="{E45FF947-6BE2-461F-A3E2-E18536134EE9}"/>
     <hyperlink ref="F4" r:id="rId2" xr:uid="{54CEF991-5998-4C51-A660-039789751FE8}"/>
+    <hyperlink ref="C7" r:id="rId3" xr:uid="{9BE7984A-ABF4-0B49-99E0-2C1387D3D204}"/>
+    <hyperlink ref="B7" r:id="rId4" xr:uid="{43AECD08-1EAC-7343-AB5E-F6FA6421C7A8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1622,17 +1677,17 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5DE38A3-6ACA-4B04-886E-9C5C02EA135E}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="64.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="52.33203125" customWidth="1"/>
   </cols>
@@ -1689,7 +1744,7 @@
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="10" t="s">
         <v>135</v>
       </c>
       <c r="C4" t="s">
@@ -1706,7 +1761,7 @@
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="8"/>
+      <c r="B5" s="10"/>
       <c r="C5" t="s">
         <v>133</v>
       </c>
@@ -1721,7 +1776,7 @@
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="10" t="s">
         <v>136</v>
       </c>
       <c r="C6" t="s">
@@ -1732,7 +1787,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B7" s="8"/>
+      <c r="B7" s="10"/>
       <c r="C7" t="s">
         <v>129</v>
       </c>
@@ -1744,7 +1799,7 @@
       <c r="A8">
         <v>6</v>
       </c>
-      <c r="B8" s="8"/>
+      <c r="B8" s="10"/>
       <c r="C8" t="s">
         <v>150</v>
       </c>
@@ -1752,10 +1807,37 @@
         <v>149</v>
       </c>
     </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B9" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="C9" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B10" s="10"/>
+      <c r="C10" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B11" s="10"/>
+      <c r="C11" t="s">
+        <v>158</v>
+      </c>
+      <c r="D11" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B12" s="10"/>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="B6:B8"/>
+    <mergeCell ref="B9:B12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1765,8 +1847,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D94782C-BCB3-5144-841C-41597F5E6A34}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1786,27 +1868,27 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="8" t="s">
         <v>136</v>
       </c>
       <c r="B2" t="s">
         <v>130</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="5" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="9"/>
+      <c r="A3" s="8"/>
       <c r="B3" t="s">
         <v>131</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="5" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="9"/>
+      <c r="A4" s="8"/>
       <c r="B4" t="s">
         <v>149</v>
       </c>
@@ -1832,6 +1914,8 @@
   <hyperlinks>
     <hyperlink ref="C4" r:id="rId1" xr:uid="{7E2BFCC3-BE60-514D-AF5E-FEB64486F0CC}"/>
     <hyperlink ref="C5" r:id="rId2" xr:uid="{ED80F6DB-712C-E843-AAE7-CC267FC0FD64}"/>
+    <hyperlink ref="C2" r:id="rId3" xr:uid="{7E3C223F-57B7-B048-9337-D61BE1BBE2AE}"/>
+    <hyperlink ref="C3" r:id="rId4" xr:uid="{ACD76D7C-030C-3A46-9D1C-7A2A9EFBA46E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add more info for crawler
Signed-off-by: Sprindy Liu <sprindy_liu@icloud.com>
</commit_message>
<xml_diff>
--- a/Documents/Readme.xlsx
+++ b/Documents/Readme.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Sprindy/program/python/python_from_0_to_0.1/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C67A7BEB-3B50-834F-9955-EF434D946EB1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A125459-3142-004A-AB71-789602298940}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1740" windowWidth="24220" windowHeight="11680" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1740" windowWidth="24220" windowHeight="11680" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Resources" sheetId="3" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Tools" sheetId="4" r:id="rId4"/>
     <sheet name="Pip" sheetId="5" r:id="rId5"/>
     <sheet name="Plot" sheetId="6" r:id="rId6"/>
+    <sheet name="爬虫" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="174">
   <si>
     <t xml:space="preserve">想高效分析客户数据, 提高查询调取数据效率，减少重复操作，提高数据的整洁和目标导向性. </t>
   </si>
@@ -522,6 +523,36 @@
   </si>
   <si>
     <t>爬虫</t>
+  </si>
+  <si>
+    <t>https://zhuanlan.zhihu.com/p/73742321</t>
+  </si>
+  <si>
+    <t>https://movie.douban.com/top250?start=0&amp;filter=</t>
+  </si>
+  <si>
+    <t>豆瓣</t>
+  </si>
+  <si>
+    <t>干货！python爬虫100个入门项目</t>
+  </si>
+  <si>
+    <t>https://www.sohu.com/a/254335921_100194747</t>
+  </si>
+  <si>
+    <t>爬虫的基本原理</t>
+  </si>
+  <si>
+    <t>https://zhuanlan.zhihu.com/p/35324806</t>
+  </si>
+  <si>
+    <t>爬虫基本原理</t>
+  </si>
+  <si>
+    <t>https://useragent.buyaocha.com</t>
+  </si>
+  <si>
+    <t>自动获取自己浏览器的UserAgent</t>
   </si>
 </sst>
 </file>
@@ -609,6 +640,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -616,11 +648,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -928,7 +959,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="7" t="s">
         <v>88</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -937,14 +968,14 @@
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="6"/>
+      <c r="A3" s="7"/>
       <c r="B3" s="1" t="s">
         <v>118</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="7" t="s">
         <v>87</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -955,12 +986,12 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="6"/>
+      <c r="A5" s="7"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="7" t="s">
         <v>89</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -969,7 +1000,7 @@
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="6"/>
+      <c r="A7" s="7"/>
       <c r="B7" s="3" t="s">
         <v>84</v>
       </c>
@@ -1049,7 +1080,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="8" t="s">
         <v>73</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1067,7 +1098,7 @@
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="7"/>
+      <c r="A3" s="8"/>
       <c r="B3" s="1" t="s">
         <v>62</v>
       </c>
@@ -1081,7 +1112,7 @@
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="7"/>
+      <c r="A4" s="8"/>
       <c r="B4" s="1" t="s">
         <v>63</v>
       </c>
@@ -1093,7 +1124,7 @@
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="7"/>
+      <c r="A5" s="8"/>
       <c r="B5" s="1" t="s">
         <v>64</v>
       </c>
@@ -1105,7 +1136,7 @@
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="7"/>
+      <c r="A6" s="8"/>
       <c r="B6" s="1" t="s">
         <v>65</v>
       </c>
@@ -1117,7 +1148,7 @@
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="7"/>
+      <c r="A7" s="8"/>
       <c r="B7" s="1" t="s">
         <v>66</v>
       </c>
@@ -1129,7 +1160,7 @@
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="8" t="s">
         <v>77</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -1143,7 +1174,7 @@
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="7"/>
+      <c r="A9" s="8"/>
       <c r="B9" s="1" t="s">
         <v>68</v>
       </c>
@@ -1155,7 +1186,7 @@
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="7"/>
+      <c r="A10" s="8"/>
       <c r="B10" s="1" t="s">
         <v>69</v>
       </c>
@@ -1167,7 +1198,7 @@
       <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="7"/>
+      <c r="A11" s="8"/>
       <c r="B11" s="1" t="s">
         <v>70</v>
       </c>
@@ -1179,7 +1210,7 @@
       <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="8" t="s">
         <v>81</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1193,7 +1224,7 @@
       <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="7"/>
+      <c r="A13" s="8"/>
       <c r="B13" s="1" t="s">
         <v>72</v>
       </c>
@@ -1550,10 +1581,10 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="C1" s="7"/>
+      <c r="C1" s="8"/>
       <c r="D1" s="1" t="s">
         <v>102</v>
       </c>
@@ -1645,7 +1676,7 @@
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="6" t="s">
         <v>161</v>
       </c>
       <c r="B7" s="5" t="s">
@@ -1679,8 +1710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5DE38A3-6ACA-4B04-886E-9C5C02EA135E}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1744,7 +1775,7 @@
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="9" t="s">
         <v>135</v>
       </c>
       <c r="C4" t="s">
@@ -1761,7 +1792,7 @@
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="10"/>
+      <c r="B5" s="9"/>
       <c r="C5" t="s">
         <v>133</v>
       </c>
@@ -1776,7 +1807,7 @@
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="9" t="s">
         <v>136</v>
       </c>
       <c r="C6" t="s">
@@ -1787,7 +1818,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B7" s="10"/>
+      <c r="B7" s="9"/>
       <c r="C7" t="s">
         <v>129</v>
       </c>
@@ -1799,7 +1830,7 @@
       <c r="A8">
         <v>6</v>
       </c>
-      <c r="B8" s="10"/>
+      <c r="B8" s="9"/>
       <c r="C8" t="s">
         <v>150</v>
       </c>
@@ -1808,7 +1839,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="9" t="s">
         <v>163</v>
       </c>
       <c r="C9" t="s">
@@ -1816,13 +1847,13 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B10" s="10"/>
+      <c r="B10" s="9"/>
       <c r="C10" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B11" s="10"/>
+      <c r="B11" s="9"/>
       <c r="C11" t="s">
         <v>158</v>
       </c>
@@ -1831,7 +1862,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B12" s="10"/>
+      <c r="B12" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1868,7 +1899,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="10" t="s">
         <v>136</v>
       </c>
       <c r="B2" t="s">
@@ -1879,7 +1910,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="8"/>
+      <c r="A3" s="10"/>
       <c r="B3" t="s">
         <v>131</v>
       </c>
@@ -1888,7 +1919,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="8"/>
+      <c r="A4" s="10"/>
       <c r="B4" t="s">
         <v>149</v>
       </c>
@@ -1919,4 +1950,69 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFDA3D0A-0E45-C54C-9A63-D129B875F61F}">
+  <dimension ref="A2:B6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="28.83203125" customWidth="1"/>
+    <col min="2" max="2" width="41" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>169</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>171</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>173</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>167</v>
+      </c>
+      <c r="B6" t="s">
+        <v>164</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{2028AD0D-89A5-8642-AE7D-2072B9BAEB12}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{7C9FC85B-A1D3-B94C-B012-BEEB5C7D5984}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{28BBB65A-DAF5-1C46-A6A6-592241FF3E17}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{DCFB8E70-13E0-614C-8DF2-3A5931A5347E}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>